<commit_message>
[specifica tecnica] Aggiornato diagramma architettura generale (.xls e .jpg)
</commit_message>
<xml_diff>
--- a/RP/Esterni/Specifica Tecnica/img/architettura generale.xlsx
+++ b/RP/Esterni/Specifica Tecnica/img/architettura generale.xlsx
@@ -48,9 +48,6 @@
     <t>CWEB 5:</t>
   </si>
   <si>
-    <t>Rispondere nuova domanda</t>
-  </si>
-  <si>
     <t>CWEB 6:</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Gestione domande e Risposte</t>
+  </si>
+  <si>
+    <t>Rispondere domanda</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -668,12 +668,12 @@
   <sheetData>
     <row r="1" spans="2:8" ht="20.25">
       <c r="B1" s="34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="35"/>
       <c r="D1" s="11"/>
       <c r="F1" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="41"/>
       <c r="H1" s="3"/>
@@ -694,7 +694,7 @@
       <c r="D3" s="14"/>
       <c r="F3" s="4"/>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="6"/>
     </row>
@@ -706,7 +706,7 @@
       <c r="D4" s="14"/>
       <c r="F4" s="4"/>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="6"/>
     </row>
@@ -726,7 +726,7 @@
       <c r="D6" s="14"/>
       <c r="F6" s="4"/>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -738,7 +738,7 @@
       <c r="D7" s="14"/>
       <c r="F7" s="4"/>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="6"/>
     </row>
@@ -753,19 +753,19 @@
     <row r="9" spans="2:8">
       <c r="F9" s="4"/>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="2:8" ht="20.25">
       <c r="B10" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="20"/>
       <c r="F10" s="4"/>
       <c r="G10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="6"/>
     </row>
@@ -785,19 +785,19 @@
       <c r="D12" s="21"/>
       <c r="F12" s="4"/>
       <c r="G12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="25"/>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="21"/>
       <c r="F13" s="4"/>
       <c r="G13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="6"/>
     </row>
@@ -826,7 +826,7 @@
       </c>
       <c r="D16" s="21"/>
       <c r="F16" s="38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="39"/>
       <c r="H16" s="27"/>
@@ -847,19 +847,19 @@
       <c r="D18" s="21"/>
       <c r="F18" s="32"/>
       <c r="G18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18" s="28"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="25"/>
       <c r="C19" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="21"/>
       <c r="F19" s="32"/>
       <c r="G19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="28"/>
     </row>
@@ -879,14 +879,14 @@
       <c r="D21" s="21"/>
       <c r="F21" s="32"/>
       <c r="G21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="28"/>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="25"/>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D22" s="21"/>
       <c r="F22" s="32"/>
@@ -911,19 +911,19 @@
       <c r="D24" s="21"/>
       <c r="F24" s="32"/>
       <c r="G24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H24" s="28"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="25"/>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="21"/>
       <c r="F25" s="32"/>
       <c r="G25" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="H25" s="28"/>
     </row>
@@ -938,24 +938,24 @@
     <row r="27" spans="2:8">
       <c r="B27" s="25"/>
       <c r="C27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27" s="21"/>
       <c r="F27" s="32"/>
       <c r="G27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H27" s="28"/>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="25"/>
       <c r="C28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="21"/>
       <c r="F28" s="32"/>
       <c r="G28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" s="28"/>
     </row>
@@ -970,19 +970,19 @@
     <row r="30" spans="2:8">
       <c r="B30" s="25"/>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" s="21"/>
       <c r="F30" s="32"/>
       <c r="G30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30" s="28"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="25"/>
       <c r="C31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="21"/>
       <c r="F31" s="32"/>
@@ -1002,7 +1002,7 @@
     <row r="33" spans="2:8">
       <c r="B33" s="25"/>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="21"/>
       <c r="F33" s="33"/>

</xml_diff>